<commit_message>
Update for teh weekly log
</commit_message>
<xml_diff>
--- a/User Information/GadaletaJakeWeeklogs.xlsx
+++ b/User Information/GadaletaJakeWeeklogs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="28">
   <si>
     <t xml:space="preserve">Items</t>
   </si>
@@ -110,6 +110,18 @@
 2. Reviewed SDS 3. Resarched lightweight web hosting with python</t>
   </si>
   <si>
+    <t xml:space="preserve">Feb 17 – 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked on the SDS Reseached further server config and test flask against python 3.8.X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Final touches to the SDS
+2. Check the SDS
+3. Work on building the basic skeleton
+4. Made a working version of flask on py 3.8x</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.
 2.
 3.
@@ -123,7 +135,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -159,6 +171,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -210,7 +228,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,6 +259,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -689,7 +711,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -1280,7 +1302,7 @@
   </sheetPr>
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -1537,8 +1559,8 @@
   </sheetPr>
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1590,7 +1612,9 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="4"/>
+      <c r="N2" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -1619,7 +1643,9 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="4"/>
+      <c r="N3" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -1648,7 +1674,9 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="4"/>
+      <c r="N4" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
@@ -1677,18 +1705,20 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
+      <c r="N5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="162" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -1707,7 +1737,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -1737,7 +1767,9 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="4"/>
+      <c r="N7" s="4" t="n">
+        <v>8</v>
+      </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
@@ -1954,7 +1986,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -2201,7 +2233,7 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
@@ -2448,7 +2480,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -2695,7 +2727,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -2942,7 +2974,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>

</xml_diff>

<commit_message>
uploading the week sheet for myself
</commit_message>
<xml_diff>
--- a/User Information/GadaletaJakeWeeklogs.xlsx
+++ b/User Information/GadaletaJakeWeeklogs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="33">
   <si>
     <t xml:space="preserve">Items</t>
   </si>
@@ -120,6 +120,24 @@
 2. Check the SDS
 3. Work on building the basic skeleton
 4. Made a working version of flask on py 3.8x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb 24 – Mar 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MWF 2, TT 1, SS 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic Server Setup, Code Compiler, Code Checker, Bundle Handler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code Compilation and Code Checking, Server Setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Wrote the complier for Java and Python (made it easy to scale to other scripting languages)
+2. Wrote the backend server information and handled the bundling
+3. Wrote the code checker in such a way that it always returns in native HTML
+4. Looked into pytests and github actions to see if we could automate some testing</t>
   </si>
   <si>
     <t xml:space="preserve">1.
@@ -135,7 +153,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -171,12 +189,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -228,7 +240,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -261,10 +273,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -288,7 +296,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -545,7 +553,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -711,7 +719,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -792,7 +800,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1049,7 +1057,7 @@
       <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1306,7 +1314,7 @@
       <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1559,11 +1567,11 @@
   </sheetPr>
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1705,20 +1713,20 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="162" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -1816,11 +1824,11 @@
   </sheetPr>
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1869,7 +1877,9 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="4"/>
+      <c r="N2" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -1898,7 +1908,9 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="4"/>
+      <c r="N3" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -1927,7 +1939,9 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="4"/>
+      <c r="N4" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
@@ -1956,7 +1970,9 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="4"/>
+      <c r="N5" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
@@ -1986,7 +2002,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -2016,7 +2032,10 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="4"/>
+      <c r="N7" s="4" t="n">
+        <f aca="false">(2 * 3) + (1 * 2) + (2 * 3)</f>
+        <v>14</v>
+      </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
@@ -2067,7 +2086,7 @@
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="16" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -2233,7 +2252,7 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
@@ -2314,7 +2333,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2480,7 +2499,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -2561,7 +2580,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2727,7 +2746,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -2808,7 +2827,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2974,7 +2993,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>

</xml_diff>